<commit_message>
Completed Working with Numeric Data in Excel
</commit_message>
<xml_diff>
--- a/03 - Entering Text/MonthlyBudget.xlsx
+++ b/03 - Entering Text/MonthlyBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/03 - Entering Text/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65231B91-1F34-4864-91E7-31FC80B9F4A1}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49B1BB65-B10C-4609-90A0-8A54488EB598}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12960" yWindow="1826" windowWidth="12343" windowHeight="6308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -378,7 +378,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -409,25 +409,70 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>1200</v>
+      </c>
+      <c r="C4">
+        <v>1200</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>135</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>150</v>
+      </c>
+      <c r="C6">
+        <v>200</v>
+      </c>
+      <c r="D6">
+        <v>125</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>300</v>
+      </c>
+      <c r="C7">
+        <v>275</v>
+      </c>
+      <c r="D7">
+        <v>350</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Completed Entering Date Values in Excel
</commit_message>
<xml_diff>
--- a/03 - Entering Text/MonthlyBudget.xlsx
+++ b/03 - Entering Text/MonthlyBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/03 - Entering Text/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49B1BB65-B10C-4609-90A0-8A54488EB598}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C66CB803-92D3-4791-8AA0-DBE492D573D4}"/>
   <bookViews>
-    <workbookView xWindow="-12960" yWindow="1826" windowWidth="12343" windowHeight="6308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13911" yWindow="1320" windowWidth="12342" windowHeight="6309" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -49,21 +49,15 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>Mar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="mmm\-yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,10 +373,14 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -392,14 +391,14 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
+      <c r="B3" s="1">
+        <v>42736</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42767</v>
+      </c>
+      <c r="D3" s="1">
+        <v>42795</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Completed Creating Basic Formulas in Excel
</commit_message>
<xml_diff>
--- a/03 - Entering Text/MonthlyBudget.xlsx
+++ b/03 - Entering Text/MonthlyBudget.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/03 - Entering Text/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C66CB803-92D3-4791-8AA0-DBE492D573D4}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C7D4C9C-72CB-43E9-B665-5A554D9C9FC2}"/>
   <bookViews>
-    <workbookView xWindow="-13911" yWindow="1320" windowWidth="12342" windowHeight="6309" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9000" yWindow="703" windowWidth="8657" windowHeight="7166" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -56,7 +67,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mmm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmm\-yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -89,7 +100,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -417,6 +428,10 @@
       <c r="D4">
         <v>1000</v>
       </c>
+      <c r="E4">
+        <f>B4+C4+D4</f>
+        <v>3400</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -431,6 +446,10 @@
       <c r="D5">
         <v>100</v>
       </c>
+      <c r="E5">
+        <f>B5+C5+D5</f>
+        <v>335</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -445,6 +464,10 @@
       <c r="D6">
         <v>125</v>
       </c>
+      <c r="E6">
+        <f>B6+C6+D6</f>
+        <v>475</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -459,6 +482,10 @@
       <c r="D7">
         <v>350</v>
       </c>
+      <c r="E7">
+        <f>B7+C7+D7</f>
+        <v>925</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -473,10 +500,26 @@
       <c r="D8">
         <v>110</v>
       </c>
+      <c r="E8">
+        <f>B8+C8+D8</f>
+        <v>310</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
+      </c>
+      <c r="B9">
+        <f>B4+B5+B6+B7+B8</f>
+        <v>1850</v>
+      </c>
+      <c r="C9">
+        <f>C4+C5+C6+C7+C8</f>
+        <v>1910</v>
+      </c>
+      <c r="D9">
+        <f>D4+D5+D6+D7+D8</f>
+        <v>1685</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Relative Versus Absolute Cell References in Formulas
</commit_message>
<xml_diff>
--- a/03 - Entering Text/MonthlyBudget.xlsx
+++ b/03 - Entering Text/MonthlyBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/03 - Entering Text/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C7D4C9C-72CB-43E9-B665-5A554D9C9FC2}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{662ADD60-8E2A-4C02-8EA9-5C519B2E29D2}"/>
   <bookViews>
-    <workbookView xWindow="-9000" yWindow="703" windowWidth="8657" windowHeight="7166" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8880" yWindow="609" windowWidth="8657" windowHeight="7165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Percent</t>
   </si>
 </sst>
 </file>
@@ -381,24 +384,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
     <col min="2" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -414,8 +419,11 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -432,8 +440,12 @@
         <f>B4+C4+D4</f>
         <v>3400</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <f>E4/$E$9</f>
+        <v>0.62442607897153357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -450,8 +462,12 @@
         <f>B5+C5+D5</f>
         <v>335</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <f>E5/$E$9</f>
+        <v>6.1524334251606978E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -468,8 +484,12 @@
         <f>B6+C6+D6</f>
         <v>475</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <f>E6/$E$9</f>
+        <v>8.7235996326905416E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -486,8 +506,12 @@
         <f>B7+C7+D7</f>
         <v>925</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <f>E7/$E$9</f>
+        <v>0.16988062442607896</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -504,8 +528,12 @@
         <f>B8+C8+D8</f>
         <v>310</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <f>E8/$E$9</f>
+        <v>5.6932966023875112E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -520,6 +548,14 @@
       <c r="D9">
         <f>D4+D5+D6+D7+D8</f>
         <v>1685</v>
+      </c>
+      <c r="E9">
+        <f>B9+C9+D9</f>
+        <v>5445</v>
+      </c>
+      <c r="F9">
+        <f>E9/$E$9</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>